<commit_message>
Excel import checkpoint; Support for linear regression isEven & isOdd added more unit tests
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sampleLogical.xlsx
+++ b/test/src/org/tms/io/sampleLogical.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3180" windowWidth="16320" windowHeight="7520" tabRatio="500"/>
+    <workbookView xWindow="9060" yWindow="10180" windowWidth="20840" windowHeight="12340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>X</t>
   </si>
@@ -55,13 +55,49 @@
   </si>
   <si>
     <t>LESS THAN</t>
+  </si>
+  <si>
+    <t>GREATER EQUAL</t>
+  </si>
+  <si>
+    <t>LESS EQUAL</t>
+  </si>
+  <si>
+    <t>IS EVEN</t>
+  </si>
+  <si>
+    <t>IS ODD</t>
+  </si>
+  <si>
+    <t>LINEAR REGRESSION</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>X VALS</t>
+  </si>
+  <si>
+    <t>Y VALS</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>r2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,6 +109,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,19 +147,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -446,9 +541,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="7"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="34" customHeight="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="34" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +564,7 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -479,14 +576,36 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:20">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -531,8 +650,37 @@
         <f>I2&lt;J2</f>
         <v>1</v>
       </c>
+      <c r="M2" t="b">
+        <f>I2&gt;=J2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <f>I2&lt;=J2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <f>ISEVEN(I2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <f>ISODD(I2)</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>2.6</v>
+      </c>
+      <c r="S2" s="4">
+        <f>SLOPE(R:R,Q:Q)</f>
+        <v>0.58418427926858219</v>
+      </c>
+      <c r="T2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:20">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -570,15 +718,44 @@
         <v>3</v>
       </c>
       <c r="K3" t="b">
-        <f t="shared" ref="K3:K5" si="5">I3&gt;J3</f>
+        <f t="shared" ref="K3:K7" si="5">I3&gt;J3</f>
         <v>0</v>
       </c>
       <c r="L3" t="b">
-        <f t="shared" ref="L3:L5" si="6">I3&lt;J3</f>
-        <v>1</v>
+        <f t="shared" ref="L3:L7" si="6">I3&lt;J3</f>
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <f t="shared" ref="M3:M7" si="7">I3&gt;=J3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <f t="shared" ref="N3:N7" si="8">I3&lt;=J3</f>
+        <v>1</v>
+      </c>
+      <c r="O3" t="b">
+        <f t="shared" ref="O3:O7" si="9">ISEVEN(I3)</f>
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <f t="shared" ref="P3:P7" si="10">ISODD(I3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="R3">
+        <v>2.8</v>
+      </c>
+      <c r="S3" s="4">
+        <f>INTERCEPT(R:R,Q:Q )</f>
+        <v>1.6842238581492919</v>
+      </c>
+      <c r="T3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:20">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -623,8 +800,37 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="M4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="R4">
+        <v>3.1</v>
+      </c>
+      <c r="S4">
+        <f>CORREL(R:R,Q:Q)</f>
+        <v>0.97405605951954211</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:20">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -669,9 +875,58 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="M5" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P5" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R5">
+        <v>4.7</v>
+      </c>
+      <c r="S5">
+        <f>RSQ(R:R,Q:Q)</f>
+        <v>0.94878520708673775</v>
+      </c>
+      <c r="T5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="Q6" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="R6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="Q7" s="7">
+        <v>6.3</v>
+      </c>
+      <c r="R7">
+        <v>5.3</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="S1:T1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>